<commit_message>
Recoded PDUFA fees to apply per FY instead of CY
</commit_message>
<xml_diff>
--- a/accelerated_approvals_vis.xlsx
+++ b/accelerated_approvals_vis.xlsx
@@ -1169,7 +1169,7 @@
         </is>
       </c>
       <c r="W7" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="X7" t="inlineStr"/>
       <c r="Y7" t="n">
@@ -1480,7 +1480,7 @@
         </is>
       </c>
       <c r="W10" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="X10" t="inlineStr"/>
       <c r="Y10" t="n">
@@ -1580,7 +1580,7 @@
         </is>
       </c>
       <c r="W11" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="X11" t="inlineStr"/>
       <c r="Y11" t="n">
@@ -1676,7 +1676,7 @@
         </is>
       </c>
       <c r="W12" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="X12" t="inlineStr"/>
       <c r="Y12" t="n">
@@ -1971,7 +1971,7 @@
         </is>
       </c>
       <c r="W15" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="X15" t="n">
         <v>9</v>
@@ -2075,7 +2075,7 @@
         </is>
       </c>
       <c r="W16" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="X16" t="n">
         <v>9</v>
@@ -2772,7 +2772,7 @@
         </is>
       </c>
       <c r="W23" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="X23" t="inlineStr"/>
       <c r="Y23" t="n">
@@ -2977,7 +2977,7 @@
         </is>
       </c>
       <c r="W25" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="X25" t="inlineStr"/>
       <c r="Y25" t="n">
@@ -3380,7 +3380,7 @@
         </is>
       </c>
       <c r="W29" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="X29" t="inlineStr"/>
       <c r="Y29" t="n">
@@ -3689,7 +3689,7 @@
         </is>
       </c>
       <c r="W32" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="X32" t="inlineStr"/>
       <c r="Y32" t="n">
@@ -4678,7 +4678,7 @@
         </is>
       </c>
       <c r="W42" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="X42" t="inlineStr"/>
       <c r="Y42" t="n">
@@ -4971,7 +4971,7 @@
         </is>
       </c>
       <c r="W45" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="X45" t="inlineStr"/>
       <c r="Y45" t="n">
@@ -5070,7 +5070,7 @@
         </is>
       </c>
       <c r="W46" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="X46" t="n">
         <v>34</v>
@@ -5172,7 +5172,7 @@
         </is>
       </c>
       <c r="W47" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="X47" t="inlineStr"/>
       <c r="Y47" t="n">
@@ -5372,7 +5372,7 @@
         </is>
       </c>
       <c r="W49" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="X49" t="n">
         <v>22</v>
@@ -5475,7 +5475,7 @@
         </is>
       </c>
       <c r="W50" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="X50" t="inlineStr"/>
       <c r="Y50" t="n">
@@ -5581,7 +5581,7 @@
         </is>
       </c>
       <c r="W51" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="X51" t="n">
         <v>28</v>
@@ -6900,7 +6900,7 @@
         </is>
       </c>
       <c r="W64" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="X64" t="inlineStr"/>
       <c r="Y64" t="n">
@@ -7000,7 +7000,7 @@
         </is>
       </c>
       <c r="W65" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="X65" t="n">
         <v>34</v>
@@ -7090,7 +7090,7 @@
         </is>
       </c>
       <c r="W66" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="X66" t="n">
         <v>30</v>
@@ -7193,7 +7193,7 @@
         </is>
       </c>
       <c r="W67" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="X67" t="inlineStr"/>
       <c r="Y67" t="n">
@@ -7401,7 +7401,7 @@
         </is>
       </c>
       <c r="W69" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="X69" t="inlineStr"/>
       <c r="Y69" t="n">
@@ -7507,7 +7507,7 @@
         </is>
       </c>
       <c r="W70" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="X70" t="inlineStr"/>
       <c r="Y70" t="n">
@@ -7608,7 +7608,7 @@
         </is>
       </c>
       <c r="W71" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="X71" t="inlineStr"/>
       <c r="Y71" t="n">
@@ -7812,7 +7812,7 @@
         </is>
       </c>
       <c r="W73" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="X73" t="inlineStr"/>
       <c r="Y73" t="n">
@@ -7916,7 +7916,7 @@
         </is>
       </c>
       <c r="W74" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="X74" t="inlineStr"/>
       <c r="Y74" t="n">
@@ -8119,7 +8119,7 @@
         </is>
       </c>
       <c r="W76" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="X76" t="inlineStr"/>
       <c r="Y76" t="n">
@@ -8226,7 +8226,7 @@
         </is>
       </c>
       <c r="W77" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="X77" t="inlineStr"/>
       <c r="Y77" t="n">
@@ -8332,7 +8332,7 @@
         </is>
       </c>
       <c r="W78" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="X78" t="inlineStr"/>
       <c r="Y78" t="n">
@@ -8432,7 +8432,7 @@
         </is>
       </c>
       <c r="W79" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="X79" t="inlineStr"/>
       <c r="Y79" t="n">
@@ -8532,7 +8532,7 @@
         </is>
       </c>
       <c r="W80" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="X80" t="n">
         <v>29</v>
@@ -8633,7 +8633,7 @@
         </is>
       </c>
       <c r="W81" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="X81" t="inlineStr"/>
       <c r="Y81" t="n">
@@ -8735,7 +8735,7 @@
         </is>
       </c>
       <c r="W82" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="X82" t="n">
         <v>28</v>
@@ -11209,7 +11209,7 @@
         </is>
       </c>
       <c r="W106" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="X106" t="inlineStr"/>
       <c r="Y106" t="n">
@@ -11721,7 +11721,7 @@
         </is>
       </c>
       <c r="W111" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="X111" t="inlineStr"/>
       <c r="Y111" t="n">
@@ -11825,7 +11825,7 @@
         </is>
       </c>
       <c r="W112" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="X112" t="inlineStr"/>
       <c r="Y112" t="n">
@@ -12036,7 +12036,7 @@
         </is>
       </c>
       <c r="W114" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="X114" t="n">
         <v>22</v>
@@ -12141,7 +12141,7 @@
         </is>
       </c>
       <c r="W115" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="X115" t="n">
         <v>47</v>
@@ -12982,7 +12982,7 @@
         </is>
       </c>
       <c r="W123" t="n">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="X123" t="n">
         <v>28</v>
@@ -13404,7 +13404,7 @@
         </is>
       </c>
       <c r="W127" t="n">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="X127" t="inlineStr"/>
       <c r="Y127" t="n">
@@ -13711,13 +13711,13 @@
         </is>
       </c>
       <c r="W130" t="n">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="X130" t="n">
         <v>28</v>
       </c>
       <c r="Y130" t="n">
-        <v>1019050</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131">
@@ -13815,13 +13815,13 @@
         </is>
       </c>
       <c r="W131" t="n">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="X131" t="n">
         <v>41</v>
       </c>
       <c r="Y131" t="n">
-        <v>1019050</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132">
@@ -14864,7 +14864,7 @@
         </is>
       </c>
       <c r="W141" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="X141" t="inlineStr"/>
       <c r="Y141" t="n">
@@ -15390,13 +15390,13 @@
         </is>
       </c>
       <c r="W146" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="X146" t="n">
         <v>52</v>
       </c>
       <c r="Y146" t="n">
-        <v>1187100</v>
+        <v>1019050</v>
       </c>
     </row>
     <row r="147">
@@ -15493,13 +15493,13 @@
         </is>
       </c>
       <c r="W147" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="X147" t="n">
         <v>16</v>
       </c>
       <c r="Y147" t="n">
-        <v>1187100</v>
+        <v>1019050</v>
       </c>
     </row>
     <row r="148">
@@ -15594,7 +15594,7 @@
         </is>
       </c>
       <c r="W148" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="X148" t="n">
         <v>38</v>
@@ -15696,7 +15696,7 @@
         </is>
       </c>
       <c r="W149" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="X149" t="n">
         <v>46</v>
@@ -15906,11 +15906,11 @@
         </is>
       </c>
       <c r="W151" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="X151" t="inlineStr"/>
       <c r="Y151" t="n">
-        <v>1187100</v>
+        <v>1019050</v>
       </c>
     </row>
     <row r="152">
@@ -16010,13 +16010,13 @@
         </is>
       </c>
       <c r="W152" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="X152" t="n">
         <v>68</v>
       </c>
       <c r="Y152" t="n">
-        <v>1187100</v>
+        <v>1019050</v>
       </c>
     </row>
     <row r="153">
@@ -17255,7 +17255,7 @@
         </is>
       </c>
       <c r="W164" t="n">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="X164" t="n">
         <v>26</v>
@@ -17361,7 +17361,7 @@
         </is>
       </c>
       <c r="W165" t="n">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="X165" t="n">
         <v>94</v>
@@ -18196,7 +18196,7 @@
         </is>
       </c>
       <c r="W173" t="n">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="X173" t="n">
         <v>69</v>
@@ -19226,7 +19226,7 @@
         </is>
       </c>
       <c r="W183" t="n">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="X183" t="inlineStr"/>
       <c r="Y183" t="n">
@@ -19327,7 +19327,7 @@
         </is>
       </c>
       <c r="W184" t="n">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="X184" t="n">
         <v>37</v>
@@ -20273,13 +20273,13 @@
         </is>
       </c>
       <c r="W193" t="n">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="X193" t="n">
         <v>91</v>
       </c>
       <c r="Y193" t="n">
-        <v>771000</v>
+        <v>920750</v>
       </c>
     </row>
     <row r="194">
@@ -21010,13 +21010,13 @@
         </is>
       </c>
       <c r="W200" t="n">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="X200" t="n">
         <v>46</v>
       </c>
       <c r="Y200" t="n">
-        <v>771000</v>
+        <v>920750</v>
       </c>
     </row>
     <row r="201">
@@ -21538,13 +21538,13 @@
         </is>
       </c>
       <c r="W205" t="n">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="X205" t="n">
         <v>123</v>
       </c>
       <c r="Y205" t="n">
-        <v>702750</v>
+        <v>771000</v>
       </c>
     </row>
     <row r="206">
@@ -21943,13 +21943,13 @@
         </is>
       </c>
       <c r="W209" t="n">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="X209" t="n">
         <v>56</v>
       </c>
       <c r="Y209" t="n">
-        <v>623600</v>
+        <v>702750</v>
       </c>
     </row>
     <row r="210">
@@ -22357,13 +22357,13 @@
         </is>
       </c>
       <c r="W213" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="X213" t="n">
         <v>105</v>
       </c>
       <c r="Y213" t="n">
-        <v>589000</v>
+        <v>623600</v>
       </c>
     </row>
     <row r="214">
@@ -22566,7 +22566,7 @@
         </is>
       </c>
       <c r="W215" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="X215" t="n">
         <v>37</v>
@@ -22669,7 +22669,7 @@
         </is>
       </c>
       <c r="W216" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="X216" t="n">
         <v>28</v>
@@ -23606,7 +23606,7 @@
         </is>
       </c>
       <c r="W225" t="n">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="X225" t="n">
         <v>16</v>
@@ -23914,7 +23914,7 @@
         </is>
       </c>
       <c r="W228" t="n">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="X228" t="n">
         <v>35</v>
@@ -24013,7 +24013,7 @@
         </is>
       </c>
       <c r="W229" t="n">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="X229" t="n">
         <v>28</v>
@@ -24115,7 +24115,7 @@
         </is>
       </c>
       <c r="W230" t="n">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="X230" t="n">
         <v>98</v>
@@ -24632,7 +24632,7 @@
         </is>
       </c>
       <c r="W235" t="n">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="X235" t="n">
         <v>28</v>
@@ -25140,13 +25140,13 @@
         </is>
       </c>
       <c r="W240" t="n">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="X240" t="n">
         <v>154</v>
       </c>
       <c r="Y240" t="n">
-        <v>286750</v>
+        <v>262200</v>
       </c>
     </row>
     <row r="241">
@@ -25637,7 +25637,7 @@
         </is>
       </c>
       <c r="W245" t="n">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="X245" t="n">
         <v>59</v>
@@ -26858,7 +26858,7 @@
         </is>
       </c>
       <c r="W257" t="n">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="X257" t="n">
         <v>47</v>
@@ -26962,7 +26962,7 @@
         </is>
       </c>
       <c r="W258" t="n">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="X258" t="n">
         <v>92</v>
@@ -27065,13 +27065,13 @@
         </is>
       </c>
       <c r="W259" t="n">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="X259" t="n">
         <v>81</v>
       </c>
       <c r="Y259" t="n">
-        <v>133803</v>
+        <v>129226</v>
       </c>
     </row>
     <row r="260">
@@ -27369,7 +27369,7 @@
         </is>
       </c>
       <c r="W262" t="n">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="X262" t="n">
         <v>78</v>
@@ -27473,7 +27473,7 @@
         </is>
       </c>
       <c r="W263" t="n">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="X263" t="n">
         <v>55</v>
@@ -28265,7 +28265,7 @@
         </is>
       </c>
       <c r="W271" t="n">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="X271" t="n">
         <v>140</v>
@@ -28678,13 +28678,13 @@
         </is>
       </c>
       <c r="W275" t="n">
-        <v>1998</v>
+        <v>1999</v>
       </c>
       <c r="X275" t="n">
         <v>68</v>
       </c>
       <c r="Y275" t="n">
-        <v>128423</v>
+        <v>136141</v>
       </c>
     </row>
     <row r="276">
@@ -28773,7 +28773,7 @@
         </is>
       </c>
       <c r="W276" t="n">
-        <v>1998</v>
+        <v>1999</v>
       </c>
       <c r="X276" t="n">
         <v>25</v>
@@ -28868,7 +28868,7 @@
         </is>
       </c>
       <c r="W277" t="n">
-        <v>1998</v>
+        <v>1999</v>
       </c>
       <c r="X277" t="n">
         <v>25</v>
@@ -28969,7 +28969,7 @@
         </is>
       </c>
       <c r="W278" t="n">
-        <v>1998</v>
+        <v>1999</v>
       </c>
       <c r="X278" t="n">
         <v>98</v>
@@ -29072,7 +29072,7 @@
         </is>
       </c>
       <c r="W279" t="n">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="X279" t="n">
         <v>118</v>
@@ -29689,7 +29689,7 @@
         </is>
       </c>
       <c r="W285" t="n">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="X285" t="n">
         <v>56</v>
@@ -29790,7 +29790,7 @@
         </is>
       </c>
       <c r="W286" t="n">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="X286" t="n">
         <v>133</v>
@@ -29998,7 +29998,7 @@
         </is>
       </c>
       <c r="W288" t="n">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="X288" t="n">
         <v>41</v>
@@ -30194,7 +30194,7 @@
         </is>
       </c>
       <c r="W290" t="n">
-        <v>1996</v>
+        <v>1997</v>
       </c>
       <c r="X290" t="n">
         <v>39</v>
@@ -30292,7 +30292,7 @@
         </is>
       </c>
       <c r="W291" t="n">
-        <v>1996</v>
+        <v>1997</v>
       </c>
       <c r="X291" t="n">
         <v>39</v>
@@ -30681,7 +30681,7 @@
         </is>
       </c>
       <c r="W295" t="n">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="X295" t="n">
         <v>29</v>
@@ -31090,7 +31090,7 @@
         </is>
       </c>
       <c r="W299" t="n">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="X299" t="n">
         <v>39</v>
@@ -31189,7 +31189,7 @@
         </is>
       </c>
       <c r="W300" t="n">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="X300" t="n">
         <v>39</v>
@@ -31907,7 +31907,7 @@
         </is>
       </c>
       <c r="W307" t="n">
-        <v>1993</v>
+        <v>1994</v>
       </c>
       <c r="X307" t="n">
         <v>18</v>
@@ -32005,7 +32005,7 @@
         </is>
       </c>
       <c r="W308" t="n">
-        <v>1992</v>
+        <v>1993</v>
       </c>
       <c r="X308" t="n">
         <v>102</v>
@@ -32101,7 +32101,7 @@
         </is>
       </c>
       <c r="W309" t="n">
-        <v>1992</v>
+        <v>1993</v>
       </c>
       <c r="X309" t="n">
         <v>102</v>
@@ -32303,7 +32303,7 @@
         </is>
       </c>
       <c r="W311" t="n">
-        <v>1991</v>
+        <v>1992</v>
       </c>
       <c r="X311" t="n">
         <v>49</v>

</xml_diff>